<commit_message>
able to successfully iterate through data table for list of products, and add them to the cart on the website with 404 and out of stock error checking
</commit_message>
<xml_diff>
--- a/Project2/Orders.xlsx
+++ b/Project2/Orders.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75AF7D46-674F-4B56-B885-1EA44164D6E0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325EC631-A360-4D0A-9C37-C32DD3B36A23}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Product</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>Laughing Lumberjack Lager</t>
-  </si>
-  <si>
-    <t>Ipoh Coff</t>
   </si>
   <si>
     <t>First Name</t>
@@ -408,7 +405,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,10 +421,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -489,7 +486,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
@@ -521,33 +518,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D2" s="1">
         <v>28787</v>
@@ -556,7 +553,7 @@
         <v>828</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more error handling; if the bot is trying to search for a product that doesn't exist, it will handle it in a specified manner instead of crashing
</commit_message>
<xml_diff>
--- a/Project2/Orders.xlsx
+++ b/Project2/Orders.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325EC631-A360-4D0A-9C37-C32DD3B36A23}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0551E5D-1A5D-42C0-8D14-1B03E17F458B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Product</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>645-2555</t>
+  </si>
+  <si>
+    <t>Ipoh Coff</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +489,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>

</xml_diff>